<commit_message>
Nozzle and CC calculations with additional ECU PCB requirements documented.
</commit_message>
<xml_diff>
--- a/Avionics/PCB/Converse ECU controller requirements.xlsx
+++ b/Avionics/PCB/Converse ECU controller requirements.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/A-OneSpace/Converse-Engine/Avionics/EngineControlUnit/PCB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/A-OneSpace/Converse-Engine/Avionics/PCB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC43C4CB-A441-6247-A6E9-8D29395F943A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C045E9-A5EE-E94F-8B72-85F3EC73CE09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16520" xr2:uid="{C4B5CCE9-66F1-694B-8BDE-ED37BD957B63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>ECU CONTROLLER REQUIREMENTS</t>
   </si>
@@ -70,6 +70,27 @@
   </si>
   <si>
     <t>Spark igniter</t>
+  </si>
+  <si>
+    <t>D-Pins</t>
+  </si>
+  <si>
+    <t>A-Pins</t>
+  </si>
+  <si>
+    <t>GND</t>
+  </si>
+  <si>
+    <t>VCC</t>
+  </si>
+  <si>
+    <t>Thermocouple</t>
+  </si>
+  <si>
+    <t>Pressure Transducer</t>
+  </si>
+  <si>
+    <t>Total Component Pins</t>
   </si>
 </sst>
 </file>
@@ -100,12 +121,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -120,15 +147,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,47 +471,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45971728-C6E2-044B-886B-FC679701BD42}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="14.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="3" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="3" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F3" s="4"/>
+      <c r="G3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -493,8 +538,13 @@
       <c r="D4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F4" s="4"/>
+      <c r="M4">
+        <f>SUM(G4:J4)*D4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -507,8 +557,25 @@
       <c r="E5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F5" s="4"/>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ref="M5:M14" si="0">SUM(G5:J5)*D5</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -518,8 +585,13 @@
       <c r="D6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F6" s="4"/>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -529,8 +601,13 @@
       <c r="D7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F7" s="4"/>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -539,6 +616,88 @@
       </c>
       <c r="D8">
         <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M14">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>